<commit_message>
Logboek bijgewerkt met afgemaakte en niet afgemaakte onderdelen
</commit_message>
<xml_diff>
--- a/TakenVerdeling.xlsx
+++ b/TakenVerdeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\GitHub\KampementKunja\KampementKunja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A847464D-85B7-44A2-B8FD-7ED62F93826F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3E49C8CE-D6DD-4203-80C8-46B29A00EF79}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="465" windowWidth="24945" windowHeight="14520" xr2:uid="{47537CA8-2881-0843-9170-AF5BC1C6BE03}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Naam</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Bijna</t>
+  </si>
+  <si>
+    <t>Datum</t>
   </si>
 </sst>
 </file>
@@ -144,8 +147,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -164,12 +168,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2C49118E-3924-004E-AB8A-F21EB763151D}" name="Tabel2" displayName="Tabel2" ref="D3:F21" totalsRowShown="0">
-  <autoFilter ref="D3:F21" xr:uid="{D5B79987-BA46-0747-8935-66C6897AB3BE}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2C49118E-3924-004E-AB8A-F21EB763151D}" name="Tabel2" displayName="Tabel2" ref="D3:G21" totalsRowShown="0">
+  <autoFilter ref="D3:G21" xr:uid="{D5B79987-BA46-0747-8935-66C6897AB3BE}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A7834271-F887-DF47-8107-54F514314533}" name="Naam"/>
     <tableColumn id="2" xr3:uid="{D1365E6A-B1D3-7949-B907-B32C76BA6D1C}" name="Taak"/>
     <tableColumn id="3" xr3:uid="{9D8E1DFA-FDCB-F946-A9AA-CEDFF9391BA7}" name="Af"/>
+    <tableColumn id="4" xr3:uid="{E671094F-DE20-41BC-8B90-F18EFFE5B4EA}" name="Datum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -472,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70333F48-4B89-7748-B2A4-CF06E484EBD1}">
-  <dimension ref="D3:F21"/>
+  <dimension ref="D3:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -483,7 +488,7 @@
     <col min="5" max="5" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -493,8 +498,11 @@
       <c r="F3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -504,8 +512,11 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>43360</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -516,7 +527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -524,10 +535,13 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>43361</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>3</v>
       </c>
@@ -535,10 +549,13 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="4:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>43362</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>3</v>
       </c>
@@ -549,7 +566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>11</v>
       </c>
@@ -560,7 +577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>11</v>
       </c>
@@ -571,7 +588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -581,8 +598,11 @@
       <c r="F11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>43361</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>11</v>
       </c>
@@ -592,8 +612,11 @@
       <c r="F12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>43361</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>11</v>
       </c>
@@ -604,7 +627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>17</v>
       </c>
@@ -615,7 +638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>17</v>
       </c>
@@ -626,7 +649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>17</v>
       </c>

</xml_diff>